<commit_message>
Added test 15 and 16 logs
</commit_message>
<xml_diff>
--- a/ML Model/docs/Parameters vs Performance of ML Model.xlsx
+++ b/ML Model/docs/Parameters vs Performance of ML Model.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Number of Examples</t>
   </si>
@@ -91,10 +91,16 @@
 Notes: Its performance is the same as coin toss.</t>
   </si>
   <si>
+    <t>Min:
+Max:
+Average Growth:
+Notes:</t>
+  </si>
+  <si>
     <t>Min: 0.009
 Max: 0.049
 Average Growth: 0.005
-So far, after 8 epoches, it rose from 0.9% to almost 5%.</t>
+Notes: So far, after 8 epoches, it rose from 0.9% to almost 5%.</t>
   </si>
 </sst>
 </file>
@@ -163,7 +169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -174,9 +180,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -480,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +509,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -735,37 +744,71 @@
         <v>8</v>
       </c>
     </row>
+    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>13</v>
+      </c>
+      <c r="B17" s="5">
+        <v>12000</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="D17" s="5">
+        <v>700</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" s="5">
         <v>12000</v>
       </c>
       <c r="C18" s="5">
-        <v>1E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="D18" s="5">
         <v>700</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" s="5">
         <v>12000</v>
       </c>
       <c r="C19" s="5">
-        <v>5.0000000000000001E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="D19" s="5">
         <v>700</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>16</v>
+      </c>
+      <c r="B20" s="5">
+        <v>12000</v>
+      </c>
+      <c r="C20" s="5">
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="D20" s="5">
+        <v>700</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Converted logs to csv files; added visualizer
</commit_message>
<xml_diff>
--- a/ML Model/docs/Parameters vs Performance of ML Model.xlsx
+++ b/ML Model/docs/Parameters vs Performance of ML Model.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Number of Examples</t>
   </si>
@@ -512,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,6 +866,23 @@
         <v>1000</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>19</v>
+      </c>
+      <c r="B23" s="5">
+        <v>30000</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="D23" s="5">
+        <v>700</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added pictures for test-19
</commit_message>
<xml_diff>
--- a/ML Model/docs/Parameters vs Performance of ML Model.xlsx
+++ b/ML Model/docs/Parameters vs Performance of ML Model.xlsx
@@ -119,18 +119,18 @@
 Notes: The test and train error avg were decreasing very rapidly; much faster than the other ones. But the accuracy was slow to progress (which could be because of the lack of data).</t>
   </si>
   <si>
-    <t xml:space="preserve">Min:
-Max:
-Num Epoche: 75
-Average Growth:
-Notes: </t>
-  </si>
-  <si>
     <t>Min: 0.01
 Max: 0.05
 Num Epoche: 49
 Average Growth: 0.0008
 Notes: The test accuracy is very bad, up and down a lot.</t>
+  </si>
+  <si>
+    <t>Min: 0.0012
+Max: 0.067
+Num Epoche: 75
+Average Growth: 0.008
+Notes: It was pretty linear</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +873,7 @@
         <v>1000</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -890,7 +890,7 @@
         <v>700</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>